<commit_message>
Added motion detection capabilities to occupancy function, reports are generated as PDFs as well as DOCX
</commit_message>
<xml_diff>
--- a/toolkit/outputs/2-energyBaseline/energyBase_summary.xlsx
+++ b/toolkit/outputs/2-energyBaseline/energyBase_summary.xlsx
@@ -414,10 +414,10 @@
         <v>3</v>
       </c>
       <c r="C2">
-        <v>0.3340188842777514</v>
+        <v>0.07066352588744917</v>
       </c>
       <c r="D2">
-        <v>0.3981489447212953</v>
+        <v>0.3901250515216378</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -428,10 +428,10 @@
         <v>4</v>
       </c>
       <c r="C3">
-        <v>0.8962641867418556</v>
+        <v>0.1493128008527864</v>
       </c>
       <c r="D3">
-        <v>0.08029191305895611</v>
+        <v>0.1342879180428377</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -442,10 +442,10 @@
         <v>5</v>
       </c>
       <c r="C4">
-        <v>0.01932791754639474</v>
+        <v>0.0308465286395686</v>
       </c>
       <c r="D4">
-        <v>0.4994323933305321</v>
+        <v>0.3770030367852095</v>
       </c>
     </row>
   </sheetData>

</xml_diff>